<commit_message>
Update app.py and questionnaire structure
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giulia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giulia/Desktop/plant_questionnaire/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6C48505-E407-EF4B-93F2-73EB6B2F667D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7035358-04B5-B643-917A-24B92098AB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1260" windowWidth="27640" windowHeight="16460" xr2:uid="{A7799B31-11A1-E849-A7C0-21A84551C890}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,32 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
-  <si>
-    <t>section</t>
-  </si>
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>input_type</t>
-  </si>
-  <si>
-    <t>options</t>
-  </si>
-  <si>
-    <t>unit_required</t>
-  </si>
-  <si>
-    <t>Plant Details</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="55">
   <si>
     <t>Select plant type</t>
   </si>
   <si>
-    <t>dropdown</t>
-  </si>
-  <si>
     <t>Incinerator,Digester</t>
   </si>
   <si>
@@ -74,22 +53,154 @@
     <t>2023,2024,2025</t>
   </si>
   <si>
-    <t>Data Entry</t>
-  </si>
-  <si>
     <t>Waste treated quantity</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Sodium bicarbonate used</t>
-  </si>
-  <si>
-    <t>Water used</t>
+    <t>Section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question </t>
+  </si>
+  <si>
+    <t>Input Type</t>
+  </si>
+  <si>
+    <t>optuons</t>
+  </si>
+  <si>
+    <t>Unit Options</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>ni</t>
+  </si>
+  <si>
+    <t>Number input</t>
+  </si>
+  <si>
+    <t>kg/year, ton/year</t>
+  </si>
+  <si>
+    <t>Unit of waste treated quantity</t>
+  </si>
+  <si>
+    <t>Lower heating value</t>
+  </si>
+  <si>
+    <t>MJ/kg</t>
+  </si>
+  <si>
+    <t>Waste composition</t>
+  </si>
+  <si>
+    <t>Text area</t>
+  </si>
+  <si>
+    <t>(no unit)</t>
+  </si>
+  <si>
+    <t>Sodium bicarbonate</t>
+  </si>
+  <si>
+    <t>kg/year, ton/year, liters/year</t>
+  </si>
+  <si>
+    <t>Activated carbon</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>Sodium hypochlorite (NaClO)</t>
+  </si>
+  <si>
+    <t>Scale and corrosion inhibitors</t>
+  </si>
+  <si>
+    <t>Alkalinizing agent</t>
+  </si>
+  <si>
+    <t>Deoxidizer</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Auxiliary fuel</t>
+  </si>
+  <si>
+    <t>Total carbon dioxide (CO2 total)</t>
+  </si>
+  <si>
+    <t>kg/year, ton/year, g/year</t>
+  </si>
+  <si>
+    <t>Biogenic carbon dioxide (CO2 bio)</t>
+  </si>
+  <si>
+    <t>% Bio CO2 from emissions analysis</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Total organic carbon (TOC)</t>
+  </si>
+  <si>
+    <t>Hydrochloric acid (HCl)</t>
+  </si>
+  <si>
+    <t>Hydrofluoric acid (HF)</t>
+  </si>
+  <si>
+    <t>Sulfur dioxide (SO2)</t>
+  </si>
+  <si>
+    <t>Nitrogen dioxide (NO2)</t>
+  </si>
+  <si>
+    <t>Ammonia (NH3)</t>
+  </si>
+  <si>
+    <t>Mercury (Hg)</t>
+  </si>
+  <si>
+    <t>Zinc (Zn)</t>
+  </si>
+  <si>
+    <t>Dioxins and furans (PCDD/PCDF)</t>
+  </si>
+  <si>
+    <t>Carbon monoxide (CO)</t>
+  </si>
+  <si>
+    <t>Total dust (&lt; 10 µm)</t>
+  </si>
+  <si>
+    <t>Polycyclic aromatic hydrocarbons (PAHs)</t>
+  </si>
+  <si>
+    <t>Cadmium (Cd)</t>
+  </si>
+  <si>
+    <t>Thallium (Tl)</t>
+  </si>
+  <si>
+    <t>Antimony (Sb)</t>
+  </si>
+  <si>
+    <t>Arsenic (As)</t>
+  </si>
+  <si>
+    <t>Lead (Pb)</t>
+  </si>
+  <si>
+    <t>Chromium (Cr)</t>
+  </si>
+  <si>
+    <t>Cobalt (Co)</t>
   </si>
 </sst>
 </file>
@@ -478,117 +589,589 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A702E8B5-BDD3-3641-807F-6C8AA8B7B2B3}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
+      <c r="A6" s="2">
+        <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>4</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>4</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>4</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>4</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>4</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>4</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>4</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>4</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>4</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed column headers and input types
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giulia/Desktop/plant_questionnaire/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7035358-04B5-B643-917A-24B92098AB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5E9474-5262-0840-9F40-E13B8F225CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1260" windowWidth="27640" windowHeight="16460" xr2:uid="{A7799B31-11A1-E849-A7C0-21A84551C890}"/>
+    <workbookView xWindow="14660" yWindow="4000" windowWidth="27640" windowHeight="16460" xr2:uid="{A7799B31-11A1-E849-A7C0-21A84551C890}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="54">
   <si>
     <t>Select plant type</t>
   </si>
@@ -65,21 +65,6 @@
     <t>Input Type</t>
   </si>
   <si>
-    <t>optuons</t>
-  </si>
-  <si>
-    <t>Unit Options</t>
-  </si>
-  <si>
-    <t>Dropdown</t>
-  </si>
-  <si>
-    <t>ni</t>
-  </si>
-  <si>
-    <t>Number input</t>
-  </si>
-  <si>
     <t>kg/year, ton/year</t>
   </si>
   <si>
@@ -95,9 +80,6 @@
     <t>Waste composition</t>
   </si>
   <si>
-    <t>Text area</t>
-  </si>
-  <si>
     <t>(no unit)</t>
   </si>
   <si>
@@ -201,6 +183,21 @@
   </si>
   <si>
     <t>Cobalt (Co)</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>unit_required</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -591,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A702E8B5-BDD3-3641-807F-6C8AA8B7B2B3}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,10 +605,10 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -622,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -639,13 +636,13 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -656,11 +653,11 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -668,14 +665,14 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -683,14 +680,14 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -698,14 +695,14 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -713,14 +710,14 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -728,14 +725,14 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -743,14 +740,14 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -758,14 +755,14 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -773,14 +770,14 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -788,14 +785,14 @@
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -803,14 +800,14 @@
         <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -818,14 +815,14 @@
         <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -833,14 +830,14 @@
         <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -848,14 +845,14 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -863,14 +860,14 @@
         <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -878,14 +875,14 @@
         <v>4</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -893,14 +890,14 @@
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -908,14 +905,14 @@
         <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -923,14 +920,14 @@
         <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -938,14 +935,14 @@
         <v>4</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -953,14 +950,14 @@
         <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -968,14 +965,14 @@
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -983,14 +980,14 @@
         <v>4</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -998,14 +995,14 @@
         <v>4</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1013,14 +1010,14 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1028,14 +1025,14 @@
         <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1043,14 +1040,14 @@
         <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1058,14 +1055,14 @@
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1073,14 +1070,14 @@
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1088,14 +1085,14 @@
         <v>4</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1103,14 +1100,14 @@
         <v>4</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1118,14 +1115,14 @@
         <v>4</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1133,14 +1130,14 @@
         <v>4</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1148,14 +1145,14 @@
         <v>4</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1163,14 +1160,14 @@
         <v>4</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>